<commit_message>
Adds MST timing comparison and improves encoding output
Compares execution times of Prim’s and Kruskal’s algorithms for Minimum Spanning Tree and updates documentation to reflect experiment details and results.

Enhances data encoding output by generating list columns for categorical features, improving readability and downstream analysis.

Facilitates algorithm selection for different graph densities and clarifies experiment outcomes.
</commit_message>
<xml_diff>
--- a/aiml lab/encoded_output.xlsx
+++ b/aiml lab/encoded_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,16 @@
           <t>moderate</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Future Dream</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Difficulty</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -531,6 +541,16 @@
       </c>
       <c r="L2" t="n">
         <v>0</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>[0, 1, 0, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>[0, 1, 0]</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -570,6 +590,16 @@
       <c r="L3" t="n">
         <v>0</v>
       </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>[0, 0, 1, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>[1, 0, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -608,6 +638,16 @@
       <c r="L4" t="n">
         <v>0</v>
       </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>[1, 0, 0, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>[0, 1, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -646,6 +686,16 @@
       <c r="L5" t="n">
         <v>0</v>
       </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0, 1, 0]</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>[1, 0, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -684,6 +734,16 @@
       <c r="L6" t="n">
         <v>0</v>
       </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 1, 0, 0]</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>[1, 0, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -722,6 +782,16 @@
       <c r="L7" t="n">
         <v>0</v>
       </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>[0, 1, 0, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>[0, 1, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -760,6 +830,16 @@
       <c r="L8" t="n">
         <v>0</v>
       </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>[0, 0, 1, 0, 0, 0]</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>[1, 0, 0]</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -797,6 +877,16 @@
       </c>
       <c r="L9" t="n">
         <v>1</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0, 0, 1]</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>[0, 0, 1]</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>